<commit_message>
Gantt chart and Architecture
</commit_message>
<xml_diff>
--- a/Artifacts/MSc Project Delivery Gantt Chart.xlsx
+++ b/Artifacts/MSc Project Delivery Gantt Chart.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roehamptonprod-my.sharepoint.com/personal/pandeym_roehampton_ac_uk/Documents/Documents/MScDataScience/Final Project/SourceCode/MscFinalProject/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD85E305-F84C-45CC-80BE-2FD3768E99E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{BD85E305-F84C-45CC-80BE-2FD3768E99E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A8684E6-4481-4290-A156-8FA7CF54D028}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{B17B6F0B-7279-475C-A991-433A432F8EF7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{B17B6F0B-7279-475C-A991-433A432F8EF7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MSc Project Gantt Chart" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -482,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,24 +493,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,9 +512,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B239E9F-D2D0-4F33-ADB7-3D8AF68A1B7E}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -933,483 +932,483 @@
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="6"/>
-      <c r="B4" s="17">
+      <c r="A4" s="22"/>
+      <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="19">
+      <c r="A5" s="23"/>
+      <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="16"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="19">
+      <c r="A7" s="23"/>
+      <c r="B7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="21"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="17">
+      <c r="A9" s="25"/>
+      <c r="B9" s="11">
         <v>2</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="18"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" s="9"/>
-      <c r="B10" s="17">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="25"/>
+      <c r="B10" s="11">
         <v>3</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="25"/>
+      <c r="B11" s="11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="18"/>
-    </row>
-    <row r="11" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="17">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="25"/>
+      <c r="B12" s="11">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="25"/>
+      <c r="B13" s="11">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="25"/>
+      <c r="B14" s="11">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="25"/>
+      <c r="B15" s="11">
+        <v>8</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="26"/>
+      <c r="B16" s="13">
+        <v>9</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="23"/>
+      <c r="B18" s="13">
+        <v>2</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="25"/>
+      <c r="B20" s="11">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" s="25"/>
+      <c r="B21" s="11">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="12"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="25"/>
+      <c r="B22" s="11">
         <v>4</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="18"/>
-    </row>
-    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="17">
+      <c r="C22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" s="25"/>
+      <c r="B23" s="11">
         <v>5</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="18"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="9"/>
-      <c r="B13" s="17">
+      <c r="C23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A24" s="25"/>
+      <c r="B24" s="11">
         <v>6</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="18"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="9"/>
-      <c r="B14" s="17">
+      <c r="C24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="26"/>
+      <c r="B25" s="13">
         <v>7</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="18"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A15" s="9"/>
-      <c r="B15" s="17">
-        <v>8</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="18"/>
-    </row>
-    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="10"/>
-      <c r="B16" s="19">
-        <v>9</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="21"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="14">
-        <v>1</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="16"/>
-    </row>
-    <row r="18" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="7"/>
-      <c r="B18" s="19">
-        <v>2</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="26"/>
-    </row>
-    <row r="19" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="14">
-        <v>1</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="16"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="9"/>
-      <c r="B20" s="17">
-        <v>2</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="18"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="9"/>
-      <c r="B21" s="17">
-        <v>3</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="18"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="9"/>
-      <c r="B22" s="17">
-        <v>4</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="18"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A23" s="9"/>
-      <c r="B23" s="17">
-        <v>5</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="18"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="9"/>
-      <c r="B24" s="17">
-        <v>6</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="27"/>
-    </row>
-    <row r="25" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="10"/>
-      <c r="B25" s="19">
-        <v>7</v>
-      </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="26"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
git ignore and initial db scripts
</commit_message>
<xml_diff>
--- a/Artifacts/MSc Project Delivery Gantt Chart.xlsx
+++ b/Artifacts/MSc Project Delivery Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roehamptonprod-my.sharepoint.com/personal/pandeym_roehampton_ac_uk/Documents/Documents/MScDataScience/Final Project/SourceCode/MscFinalProject/Artifacts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roehamptonprod-my.sharepoint.com/personal/pandeym_roehampton_ac_uk/Documents/Documents/MScDataScience/Projects/MSc_Project/SourceCode/MscFinalProject/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{BD85E305-F84C-45CC-80BE-2FD3768E99E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A8684E6-4481-4290-A156-8FA7CF54D028}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{BD85E305-F84C-45CC-80BE-2FD3768E99E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD23F5A-8867-4113-AE31-778E0B05D71E}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{B17B6F0B-7279-475C-A991-433A432F8EF7}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{B17B6F0B-7279-475C-A991-433A432F8EF7}"/>
   </bookViews>
   <sheets>
     <sheet name="MSc Project Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -547,6 +547,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -869,25 +873,25 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="38.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.9375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.703125" customWidth="1"/>
+    <col min="3" max="3" width="38.17578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.05859375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.46875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.9375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.87890625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -922,7 +926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -963,7 +967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="21" t="s">
         <v>22</v>
       </c>
@@ -975,8 +979,8 @@
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -984,7 +988,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="22"/>
       <c r="B4" s="11">
         <v>2</v>
@@ -1003,7 +1007,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="23"/>
       <c r="B5" s="13">
         <v>3</v>
@@ -1022,7 +1026,7 @@
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
@@ -1043,7 +1047,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="23"/>
       <c r="B7" s="13">
         <v>2</v>
@@ -1062,7 +1066,7 @@
       <c r="L7" s="14"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>25</v>
       </c>
@@ -1083,7 +1087,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="25"/>
       <c r="B9" s="11">
         <v>2</v>
@@ -1102,7 +1106,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="25"/>
       <c r="B10" s="11">
         <v>3</v>
@@ -1112,16 +1116,16 @@
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="18"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="7"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="25"/>
       <c r="B11" s="11">
         <v>4</v>
@@ -1140,7 +1144,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="25"/>
       <c r="B12" s="11">
         <v>5</v>
@@ -1159,7 +1163,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="25"/>
       <c r="B13" s="11">
         <v>6</v>
@@ -1178,7 +1182,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" s="25"/>
       <c r="B14" s="11">
         <v>7</v>
@@ -1197,7 +1201,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="25"/>
       <c r="B15" s="11">
         <v>8</v>
@@ -1216,7 +1220,7 @@
       <c r="L15" s="18"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="26"/>
       <c r="B16" s="13">
         <v>9</v>
@@ -1235,7 +1239,7 @@
       <c r="L16" s="16"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A17" s="21" t="s">
         <v>26</v>
       </c>
@@ -1256,7 +1260,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="23"/>
       <c r="B18" s="13">
         <v>2</v>
@@ -1275,7 +1279,7 @@
       <c r="L18" s="14"/>
       <c r="M18" s="19"/>
     </row>
-    <row r="19" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="24" t="s">
         <v>27</v>
       </c>
@@ -1296,7 +1300,7 @@
       <c r="L19" s="9"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A20" s="25"/>
       <c r="B20" s="11">
         <v>2</v>
@@ -1315,7 +1319,7 @@
       <c r="L20" s="7"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A21" s="25"/>
       <c r="B21" s="11">
         <v>3</v>
@@ -1334,7 +1338,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A22" s="25"/>
       <c r="B22" s="11">
         <v>4</v>
@@ -1353,7 +1357,7 @@
       <c r="L22" s="18"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A23" s="25"/>
       <c r="B23" s="11">
         <v>5</v>
@@ -1372,7 +1376,7 @@
       <c r="L23" s="18"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A24" s="25"/>
       <c r="B24" s="11">
         <v>6</v>
@@ -1391,7 +1395,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="20"/>
     </row>
-    <row r="25" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="26"/>
       <c r="B25" s="13">
         <v>7</v>

</xml_diff>